<commit_message>
with new goal of KTH map
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/GoalConfig.xlsx
+++ b/AD-EYE/TA/GoalConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -135,12 +135,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -152,18 +152,18 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,7 +179,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-8.99</v>
+        <v>255.29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,7 +187,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>136.18</v>
+        <v>-514.31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,7 +219,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0</v>
+        <v>0.481</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,7 +227,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0</v>
+        <v>-0.877</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,7 +241,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
ressources folder added and open scenario world
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/GoalConfig.xlsx
+++ b/AD-EYE/TA/GoalConfig.xlsx
@@ -153,17 +153,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,7 +178,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>255.29</v>
+        <v>37.39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,7 +186,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-514.31</v>
+        <v>69.49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,7 +202,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,7 +210,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>0.327</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,7 +218,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.481</v>
+        <v>0.327</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,7 +226,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-0.877</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
settings to test experiment A length and experiment B .xosc correction, add pedestrian to action
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/GoalConfig.xlsx
+++ b/AD-EYE/TA/GoalConfig.xlsx
@@ -153,17 +153,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,7 +178,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>255.29</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,7 +186,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-514.31</v>
+        <v>-259</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,7 +202,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0</v>
+        <v>0.343</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,7 +210,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>-0.618</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,7 +218,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.481</v>
+        <v>0.343</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,7 +226,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-0.877</v>
+        <v>-0.618</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
set goal for experimentA
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/GoalConfig.xlsx
+++ b/AD-EYE/TA/GoalConfig.xlsx
@@ -153,10 +153,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
@@ -178,7 +178,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>88</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,7 +186,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-259</v>
+        <v>-339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -202,7 +202,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.343</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,7 +210,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>-0.618</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,7 +218,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.343</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,7 +226,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-0.618</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>